<commit_message>
Update max and min
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\simple_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382A1052-863F-474F-9771-39731397D35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3FEACB-EC38-45EA-8F4E-E9137E5740DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Data 1</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Data 2</t>
+    <t>Data1</t>
   </si>
   <si>
-    <t>Data 3</t>
+    <t>Data2</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Data3</t>
   </si>
 </sst>
 </file>
@@ -368,23 +368,23 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>